<commit_message>
1. Correct some uncorrect label on main page 2. Changed PSLExample.xlsx - structure, set nonshown 0, pin headers and columns 3. Change fonts and styles in WritePSLController Changes in WriteEASController not importent and made accidentally
</commit_message>
<xml_diff>
--- a/src/main/resources/PSLExample.xlsx
+++ b/src/main/resources/PSLExample.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr showInkAnnotation="0" codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDEA\Idea Projects\sldocs\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SLDOCS\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45AB150-8307-4F5A-8417-2490719C52D2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85913E8A-8F13-40C4-9863-871AFB20CDB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Норматив_2020_2021" sheetId="67" r:id="rId1"/>
+    <sheet name="Норматив" sheetId="67" r:id="rId1"/>
     <sheet name="ВикладачПриклад" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">ВикладачПриклад!$A$1:$T$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">ВикладачПриклад!$A$1:$T$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Завідувач кафедри</t>
   </si>
@@ -98,32 +105,26 @@
     <t>Усього</t>
   </si>
   <si>
-    <t>Норматив</t>
-  </si>
-  <si>
-    <t>Викладач 12</t>
-  </si>
-  <si>
-    <t>осінь</t>
-  </si>
-  <si>
-    <t>stuff</t>
-  </si>
-  <si>
-    <t>ПЛАН УЧБОВОГО НАВАНТАЖЕННЯ ВИКЛАДАЧА</t>
-  </si>
-  <si>
     <t>Дисципліна</t>
   </si>
   <si>
     <t>Група</t>
+  </si>
+  <si>
+    <t>Кафедра</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Викладач </t>
+  </si>
+  <si>
+    <t>ПЛАН НАВЧАЛЬНОГО НАВАНТАЖЕННЯ ВИКЛАДАЧА НА 2022/2023 НАВЧАЛЬНИЙ РІК</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="63"/>
@@ -178,10 +179,18 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="63"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="63"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -193,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -217,55 +226,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -280,7 +250,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -293,99 +263,6 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -399,49 +276,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Обычный 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
@@ -813,44 +680,44 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="21" width="9.42578125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="6.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="21" width="9.44140625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4">
         <v>1.5</v>
       </c>
-      <c r="D1" s="10">
+      <c r="D1" s="4">
         <v>1.25</v>
       </c>
-      <c r="E1" s="10">
+      <c r="E1" s="4">
         <v>1</v>
       </c>
-      <c r="F1" s="10">
+      <c r="F1" s="4">
         <v>0.5</v>
       </c>
-      <c r="G1" s="10">
+      <c r="G1" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="11" customFormat="1">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:7" s="5" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="3">
         <f>$C$1*E2</f>
         <v>720</v>
@@ -859,7 +726,7 @@
         <f>$D$1*E2</f>
         <v>600</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="4">
         <v>480</v>
       </c>
       <c r="F2" s="3">
@@ -1124,29 +991,30 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="56" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="45" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
-    <col min="5" max="20" width="9.42578125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="6.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="1" customWidth="1"/>
+    <col min="5" max="20" width="9.44140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.5" thickBot="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7"/>
+    <row r="1" spans="1:23">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E1" s="8"/>
@@ -1164,140 +1032,147 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
-      <c r="T1" s="9"/>
-    </row>
-    <row r="3" spans="1:20" ht="19.5" thickBot="1">
-      <c r="A3" s="16" t="s">
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:23" ht="18.600000000000001" thickBot="1">
+      <c r="A3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="14"/>
+    </row>
+    <row r="4" spans="1:23" ht="145.80000000000001" thickBot="1">
+      <c r="A4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="T3" s="25"/>
-    </row>
-    <row r="4" spans="1:20" ht="150.75">
-      <c r="A4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="19.5" thickBot="1">
-      <c r="A5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="21"/>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-    </row>
-    <row r="17" spans="3:23">
-      <c r="W17" s="15"/>
-    </row>
-    <row r="25" spans="3:23">
-      <c r="U25" s="14"/>
-    </row>
-    <row r="29" spans="3:23">
+    <row r="15" spans="1:23">
+      <c r="W15" s="7"/>
+    </row>
+    <row r="23" spans="3:21">
+      <c r="U23" s="6"/>
+    </row>
+    <row r="27" spans="3:21">
+      <c r="C27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" spans="3:21">
+      <c r="C28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="6"/>
+    </row>
+    <row r="29" spans="3:21">
       <c r="C29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1316,7 +1191,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="3:23">
+    <row r="30" spans="3:21">
       <c r="C30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1334,51 +1209,9 @@
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
-      <c r="U30" s="14"/>
-    </row>
-    <row r="31" spans="3:23">
-      <c r="C31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-    </row>
-    <row r="32" spans="3:23">
-      <c r="C32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A6:T6"/>
-  </mergeCells>
-  <conditionalFormatting sqref="U25">
+  <conditionalFormatting sqref="U23">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -1387,6 +1220,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" scale="48" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SLD-015 final changes in progress
</commit_message>
<xml_diff>
--- a/src/main/resources/PSLExample.xlsx
+++ b/src/main/resources/PSLExample.xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr showInkAnnotation="0" codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SLDOCS\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDEA\Idea Projects\sldocs\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85913E8A-8F13-40C4-9863-871AFB20CDB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7331CC0F-8FDA-4715-8FF7-A1EDEFE3DD84}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Норматив" sheetId="67" r:id="rId1"/>
-    <sheet name="ВикладачПриклад" sheetId="7" r:id="rId2"/>
+    <sheet name="Кафедра" sheetId="69" r:id="rId1"/>
+    <sheet name="Норматив" sheetId="67" r:id="rId2"/>
+    <sheet name="ВикладачПриклад" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">ВикладачПриклад!$A$1:$T$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">ВикладачПриклад!$A$1:$T$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Кафедра!$A$1:$F$61</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Завідувач кафедри</t>
   </si>
@@ -118,13 +113,64 @@
   </si>
   <si>
     <t>ПЛАН НАВЧАЛЬНОГО НАВАНТАЖЕННЯ ВИКЛАДАЧА НА 2022/2023 НАВЧАЛЬНИЙ РІК</t>
+  </si>
+  <si>
+    <t>ЗВЕДЕНЕ НАВЧАЛЬНЕ НАВАНТАЖЕННЯ кафедри ПРОГРАМНОЇ ІНЖЕНЕРІЇ та ІНТЕЛЕКТУАЛЬНИХ УПРАВЛІННЯ на 2022/2023 навч.рік</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Станом на 24.01.2023 </t>
+  </si>
+  <si>
+    <t>№ з/п</t>
+  </si>
+  <si>
+    <t>Посада</t>
+  </si>
+  <si>
+    <t>Штат /сумісництво</t>
+  </si>
+  <si>
+    <t>Викладач</t>
+  </si>
+  <si>
+    <t>Навантеження</t>
+  </si>
+  <si>
+    <t>осінь 2022</t>
+  </si>
+  <si>
+    <t>весна 2023</t>
+  </si>
+  <si>
+    <t>магістри, кількість</t>
+  </si>
+  <si>
+    <t>магістри, годин</t>
+  </si>
+  <si>
+    <t>бакалаври, кількість</t>
+  </si>
+  <si>
+    <t>бакалаври, годин</t>
+  </si>
+  <si>
+    <t>СУМА, годин</t>
+  </si>
+  <si>
+    <t>План (из расчета 600)</t>
+  </si>
+  <si>
+    <t>Pізниця</t>
+  </si>
+  <si>
+    <t>Примітка</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color indexed="63"/>
@@ -193,16 +239,136 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4F6228"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4F6228"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -270,13 +436,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -306,13 +486,146 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+  <cellStyles count="4">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{12995EFD-D4BB-4A29-A864-07FD92C58D65}"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Обычный 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -676,25 +989,1321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE32BB9B-E843-47F3-88FA-7916C5867BD9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AMF68"/>
+  <sheetViews>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="31" customWidth="1"/>
+    <col min="6" max="7" width="14.42578125" style="33" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="33" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="33" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="33" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="33" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="33" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="34" customWidth="1"/>
+    <col min="15" max="15" width="27" style="33" customWidth="1"/>
+    <col min="16" max="1020" width="9.140625" style="33"/>
+    <col min="1021" max="16384" width="9.140625" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" s="20" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+    </row>
+    <row r="2" spans="1:47" s="20" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+    </row>
+    <row r="3" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A3" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+    </row>
+    <row r="4" spans="1:47" s="20" customFormat="1" ht="56.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="39"/>
+    </row>
+    <row r="6" spans="1:47" s="26" customFormat="1" ht="18.75">
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="47"/>
+    </row>
+    <row r="7" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="44"/>
+    </row>
+    <row r="8" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="44"/>
+    </row>
+    <row r="9" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="44"/>
+    </row>
+    <row r="10" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="44"/>
+    </row>
+    <row r="11" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="44"/>
+    </row>
+    <row r="12" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="26"/>
+      <c r="AL12" s="26"/>
+      <c r="AM12" s="26"/>
+      <c r="AN12" s="26"/>
+      <c r="AO12" s="26"/>
+      <c r="AP12" s="26"/>
+      <c r="AQ12" s="26"/>
+      <c r="AR12" s="26"/>
+      <c r="AS12" s="26"/>
+      <c r="AT12" s="26"/>
+      <c r="AU12" s="26"/>
+    </row>
+    <row r="13" spans="1:47" s="27" customFormat="1" ht="18.75">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="20"/>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="20"/>
+      <c r="AI13" s="20"/>
+      <c r="AJ13" s="20"/>
+      <c r="AK13" s="20"/>
+      <c r="AL13" s="20"/>
+      <c r="AM13" s="20"/>
+      <c r="AN13" s="20"/>
+      <c r="AO13" s="20"/>
+      <c r="AP13" s="20"/>
+      <c r="AQ13" s="20"/>
+      <c r="AR13" s="20"/>
+      <c r="AS13" s="20"/>
+      <c r="AT13" s="20"/>
+      <c r="AU13" s="20"/>
+    </row>
+    <row r="14" spans="1:47" s="27" customFormat="1" ht="18.75">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="20"/>
+      <c r="AH14" s="20"/>
+      <c r="AI14" s="20"/>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="20"/>
+      <c r="AL14" s="20"/>
+      <c r="AM14" s="20"/>
+      <c r="AN14" s="20"/>
+      <c r="AO14" s="20"/>
+      <c r="AP14" s="20"/>
+      <c r="AQ14" s="20"/>
+      <c r="AR14" s="20"/>
+      <c r="AS14" s="20"/>
+      <c r="AT14" s="20"/>
+      <c r="AU14" s="20"/>
+    </row>
+    <row r="15" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="44"/>
+    </row>
+    <row r="16" spans="1:47" s="27" customFormat="1" ht="18.75">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+      <c r="AI16" s="20"/>
+      <c r="AJ16" s="20"/>
+      <c r="AK16" s="20"/>
+      <c r="AL16" s="20"/>
+      <c r="AM16" s="20"/>
+      <c r="AN16" s="20"/>
+      <c r="AO16" s="20"/>
+      <c r="AP16" s="20"/>
+      <c r="AQ16" s="20"/>
+      <c r="AR16" s="20"/>
+      <c r="AS16" s="20"/>
+      <c r="AT16" s="20"/>
+      <c r="AU16" s="20"/>
+    </row>
+    <row r="17" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="26"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="26"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="26"/>
+      <c r="AB17" s="26"/>
+      <c r="AC17" s="26"/>
+      <c r="AD17" s="26"/>
+      <c r="AE17" s="26"/>
+      <c r="AF17" s="26"/>
+      <c r="AG17" s="26"/>
+      <c r="AH17" s="26"/>
+      <c r="AI17" s="26"/>
+      <c r="AJ17" s="26"/>
+      <c r="AK17" s="26"/>
+      <c r="AL17" s="26"/>
+      <c r="AM17" s="26"/>
+      <c r="AN17" s="26"/>
+      <c r="AO17" s="26"/>
+      <c r="AP17" s="26"/>
+      <c r="AQ17" s="26"/>
+      <c r="AR17" s="26"/>
+      <c r="AS17" s="26"/>
+      <c r="AT17" s="26"/>
+      <c r="AU17" s="26"/>
+    </row>
+    <row r="18" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="44"/>
+    </row>
+    <row r="19" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="44"/>
+    </row>
+    <row r="20" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="44"/>
+    </row>
+    <row r="21" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="44"/>
+    </row>
+    <row r="22" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="44"/>
+    </row>
+    <row r="23" spans="1:47" s="26" customFormat="1" ht="18.75">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="47"/>
+    </row>
+    <row r="24" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="44"/>
+    </row>
+    <row r="25" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="44"/>
+    </row>
+    <row r="26" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="44"/>
+    </row>
+    <row r="27" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="48"/>
+      <c r="O27" s="44"/>
+    </row>
+    <row r="28" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="44"/>
+    </row>
+    <row r="29" spans="1:47" s="20" customFormat="1" ht="18.75">
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="48"/>
+      <c r="O29" s="44"/>
+    </row>
+    <row r="30" spans="1:47" s="28" customFormat="1" ht="18.75">
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="51"/>
+    </row>
+    <row r="31" spans="1:47" s="28" customFormat="1" ht="18.75">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="51"/>
+    </row>
+    <row r="32" spans="1:47" s="28" customFormat="1" ht="18.75">
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="51"/>
+    </row>
+    <row r="33" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="44"/>
+    </row>
+    <row r="34" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="48"/>
+      <c r="O34" s="44"/>
+    </row>
+    <row r="35" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="44"/>
+    </row>
+    <row r="36" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="48"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="48"/>
+      <c r="O36" s="44"/>
+    </row>
+    <row r="37" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="44"/>
+    </row>
+    <row r="38" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="48"/>
+      <c r="O38" s="44"/>
+    </row>
+    <row r="39" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="44"/>
+    </row>
+    <row r="40" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="48"/>
+      <c r="O40" s="44"/>
+    </row>
+    <row r="41" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="44"/>
+    </row>
+    <row r="42" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="48"/>
+      <c r="O42" s="44"/>
+    </row>
+    <row r="43" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="44"/>
+    </row>
+    <row r="44" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="44"/>
+    </row>
+    <row r="45" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="44"/>
+    </row>
+    <row r="46" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="44"/>
+    </row>
+    <row r="47" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="44"/>
+    </row>
+    <row r="48" spans="1:15" s="20" customFormat="1" ht="18.75">
+      <c r="A48" s="44"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="48"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="44"/>
+    </row>
+    <row r="49" spans="1:15" s="28" customFormat="1" ht="18.75">
+      <c r="A49" s="44"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="51"/>
+    </row>
+    <row r="50" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A50" s="44"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="50"/>
+    </row>
+    <row r="51" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="50"/>
+    </row>
+    <row r="52" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="50"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="48"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="50"/>
+    </row>
+    <row r="53" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A53" s="44"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="44"/>
+      <c r="L53" s="48"/>
+      <c r="M53" s="48"/>
+      <c r="N53" s="48"/>
+      <c r="O53" s="50"/>
+    </row>
+    <row r="54" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="50"/>
+      <c r="K54" s="44"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="48"/>
+      <c r="N54" s="48"/>
+      <c r="O54" s="50"/>
+    </row>
+    <row r="55" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="50"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="48"/>
+      <c r="M55" s="48"/>
+      <c r="N55" s="48"/>
+      <c r="O55" s="50"/>
+    </row>
+    <row r="56" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="50"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="48"/>
+      <c r="M56" s="48"/>
+      <c r="N56" s="48"/>
+      <c r="O56" s="50"/>
+    </row>
+    <row r="57" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A57" s="44"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="45"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="50"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="48"/>
+      <c r="M57" s="48"/>
+      <c r="N57" s="48"/>
+      <c r="O57" s="50"/>
+    </row>
+    <row r="58" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A58" s="44"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="50"/>
+      <c r="K58" s="44"/>
+      <c r="L58" s="48"/>
+      <c r="M58" s="48"/>
+      <c r="N58" s="48"/>
+      <c r="O58" s="50"/>
+    </row>
+    <row r="59" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A59" s="44"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="50"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="50"/>
+    </row>
+    <row r="60" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="50"/>
+      <c r="H60" s="50"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="50"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="48"/>
+      <c r="M60" s="48"/>
+      <c r="N60" s="48"/>
+      <c r="O60" s="50"/>
+    </row>
+    <row r="61" spans="1:15" s="29" customFormat="1" ht="18.75">
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="50"/>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" s="52"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="55"/>
+      <c r="L62" s="48"/>
+      <c r="M62" s="56"/>
+      <c r="N62" s="56"/>
+      <c r="O62" s="55"/>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="D64" s="32"/>
+    </row>
+    <row r="65" spans="4:5">
+      <c r="D65" s="32"/>
+    </row>
+    <row r="68" spans="4:5">
+      <c r="D68" s="35"/>
+      <c r="E68" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F3:O3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N5:N61">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.43333333333333302" right="3.9583333333333297E-2" top="0.31527777777777799" bottom="0.23611111111111099" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" fitToHeight="2" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="6.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="21" width="9.44140625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="6.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="21" width="9.42578125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4">
@@ -713,7 +2322,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -738,7 +2347,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -985,7 +2594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Лист8">
     <tabColor rgb="FF92D050"/>
@@ -997,17 +2606,17 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="45" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" style="1" customWidth="1"/>
-    <col min="5" max="20" width="9.44140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="5" max="20" width="9.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -1037,7 +2646,7 @@
     <row r="2" spans="1:23">
       <c r="A2" s="18"/>
     </row>
-    <row r="3" spans="1:23" ht="18.600000000000001" thickBot="1">
+    <row r="3" spans="1:23" ht="19.5" thickBot="1">
       <c r="A3" s="17" t="s">
         <v>27</v>
       </c>
@@ -1065,7 +2674,7 @@
       <c r="S3" s="15"/>
       <c r="T3" s="14"/>
     </row>
-    <row r="4" spans="1:23" ht="145.80000000000001" thickBot="1">
+    <row r="4" spans="1:23" ht="152.25" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
@@ -1212,10 +2821,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="U23">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>47</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>